<commit_message>
fixed date selection to be more straightforward. Added Excel closing to remove open file issue
</commit_message>
<xml_diff>
--- a/Summary Report.xlsx
+++ b/Summary Report.xlsx
@@ -518,6 +518,7 @@
         <v>0</v>
       </c>
       <c r="N2">
+        <f>SUM(B2:M2)</f>
         <v>0</v>
       </c>
     </row>
@@ -562,6 +563,7 @@
         <v>0</v>
       </c>
       <c r="N3">
+        <f>SUM(B3:M3)</f>
         <v>0</v>
       </c>
     </row>
@@ -606,6 +608,7 @@
         <v>0</v>
       </c>
       <c r="N4">
+        <f>SUM(B4:M4)</f>
         <v>0</v>
       </c>
     </row>
@@ -650,6 +653,7 @@
         <v>0</v>
       </c>
       <c r="N5">
+        <f>SUM(B5:M5)</f>
         <v>0</v>
       </c>
     </row>
@@ -694,6 +698,7 @@
         <v>0</v>
       </c>
       <c r="N6">
+        <f>SUM(B6:M6)</f>
         <v>0</v>
       </c>
     </row>
@@ -702,42 +707,55 @@
         <v>18</v>
       </c>
       <c r="B7">
+        <f>SUM(B2:B6)</f>
         <v>0</v>
       </c>
       <c r="C7">
+        <f>SUM(C2:C6)</f>
         <v>0</v>
       </c>
       <c r="D7">
+        <f>SUM(D2:D6)</f>
         <v>0</v>
       </c>
       <c r="E7">
+        <f>SUM(E2:E6)</f>
         <v>0</v>
       </c>
       <c r="F7">
+        <f>SUM(F2:F6)</f>
         <v>0</v>
       </c>
       <c r="G7">
+        <f>SUM(G2:G6)</f>
         <v>0</v>
       </c>
       <c r="H7">
+        <f>SUM(H2:H6)</f>
         <v>0</v>
       </c>
       <c r="I7">
+        <f>SUM(I2:I6)</f>
         <v>0</v>
       </c>
       <c r="J7">
+        <f>SUM(J2:J6)</f>
         <v>0</v>
       </c>
       <c r="K7">
+        <f>SUM(K2:K6)</f>
         <v>0</v>
       </c>
       <c r="L7">
+        <f>SUM(L2:L6)</f>
         <v>0</v>
       </c>
       <c r="M7">
+        <f>SUM(M2:M6)</f>
         <v>0</v>
       </c>
       <c r="N7">
+        <f>SUM(N2:N6)</f>
         <v>0</v>
       </c>
     </row>
@@ -1172,6 +1190,7 @@
         <v>0</v>
       </c>
       <c r="N2">
+        <f>SUM(B2:M2)</f>
         <v>0</v>
       </c>
     </row>
@@ -1189,10 +1208,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3491</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>3491</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1216,6 +1235,7 @@
         <v>0</v>
       </c>
       <c r="N3">
+        <f>SUM(B3:M3)</f>
         <v>0</v>
       </c>
     </row>
@@ -1233,10 +1253,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2875</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2875</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1260,6 +1280,7 @@
         <v>0</v>
       </c>
       <c r="N4">
+        <f>SUM(B4:M4)</f>
         <v>0</v>
       </c>
     </row>
@@ -1304,6 +1325,7 @@
         <v>0</v>
       </c>
       <c r="N5">
+        <f>SUM(B5:M5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1321,10 +1343,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>953.3085</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>953.3085</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1348,6 +1370,7 @@
         <v>0</v>
       </c>
       <c r="N6">
+        <f>SUM(B6:M6)</f>
         <v>0</v>
       </c>
     </row>
@@ -1356,42 +1379,55 @@
         <v>18</v>
       </c>
       <c r="B7">
+        <f>SUM(B2:B6)</f>
         <v>0</v>
       </c>
       <c r="C7">
+        <f>SUM(C2:C6)</f>
         <v>0</v>
       </c>
       <c r="D7">
+        <f>SUM(D2:D6)</f>
         <v>0</v>
       </c>
       <c r="E7">
+        <f>SUM(E2:E6)</f>
         <v>0</v>
       </c>
       <c r="F7">
+        <f>SUM(F2:F6)</f>
         <v>0</v>
       </c>
       <c r="G7">
+        <f>SUM(G2:G6)</f>
         <v>0</v>
       </c>
       <c r="H7">
+        <f>SUM(H2:H6)</f>
         <v>0</v>
       </c>
       <c r="I7">
+        <f>SUM(I2:I6)</f>
         <v>0</v>
       </c>
       <c r="J7">
+        <f>SUM(J2:J6)</f>
         <v>0</v>
       </c>
       <c r="K7">
+        <f>SUM(K2:K6)</f>
         <v>0</v>
       </c>
       <c r="L7">
+        <f>SUM(L2:L6)</f>
         <v>0</v>
       </c>
       <c r="M7">
+        <f>SUM(M2:M6)</f>
         <v>0</v>
       </c>
       <c r="N7">
+        <f>SUM(N2:N6)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>